<commit_message>
Can now load XML file
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C989E93-1F01-4EE6-AA45-30C775A2DF03}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC20BA5E-6905-41C8-B09E-EFB71394AA5F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
@@ -29,8 +29,22 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{7A79F9D7-CD02-4FDF-B5CF-C3AF89855961}" name="Schema" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" xr16:uid="{751CB7F7-EAA6-48E0-9A1F-CDEDF00F9B68}" name="Schema1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="3" xr16:uid="{7C2187DD-9C47-4A30-8977-D2530993B475}" name="Schema2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
   <si>
     <t>Voornaam</t>
   </si>
@@ -41,15 +55,6 @@
     <t>Bericht</t>
   </si>
   <si>
-    <t>Relevant</t>
-  </si>
-  <si>
-    <t>JA</t>
-  </si>
-  <si>
-    <t>NEE</t>
-  </si>
-  <si>
     <t>Is dit al opgelost?</t>
   </si>
   <si>
@@ -291,6 +296,9 @@
   </si>
   <si>
     <t>van den Heuvel</t>
+  </si>
+  <si>
+    <t>POI</t>
   </si>
 </sst>
 </file>
@@ -326,13 +334,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -343,6 +359,71 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema3">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="data-set">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" name="NotificationCollection" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" name="Notifications" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Notification" form="unqualified">
+                          <xsd:complexType>
+                            <xsd:sequence minOccurs="0">
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Voornaam" form="unqualified"/>
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Achternaam" form="unqualified"/>
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Bericht" form="unqualified"/>
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="POI" form="unqualified"/>
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mediaplatform" form="unqualified"/>
+                            </xsd:sequence>
+                          </xsd:complexType>
+                        </xsd:element>
+                      </xsd:sequence>
+                    </xsd:complexType>
+                  </xsd:element>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="3" Name="data-set_toewijzing" RootElement="data-set" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+  </Map>
+</MapInfo>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="3">
+  <autoFilter ref="A1:E26" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Voornaam" name="Voornaam">
+      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Voornaam" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{E5E2E653-7318-47D2-9903-41062D660767}" uniqueName="Achternaam" name="Achternaam">
+      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Achternaam" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Bericht" name="Bericht">
+      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Bericht" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="POI" name="POI" dataDxfId="0">
+      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Mediaplatform" name="Mediaplatform">
+      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Mediaplatform" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -645,14 +726,15 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="9" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,439 +747,442 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D12" s="1">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>18</v>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added standard images and Updated XML file
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043F38B1-5C66-4A0E-849B-D32CAB9939CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C72251-A8F3-4390-80CF-C478EF0CD6E8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
@@ -40,18 +40,18 @@
   <connection id="3" xr16:uid="{7C2187DD-9C47-4A30-8977-D2530993B475}" name="Schema2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="4" xr16:uid="{0ED1EF86-BBAE-4CC0-9C3B-F4D02FDB3F56}" name="Schema3" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Voornaam</t>
   </si>
   <si>
-    <t>Achternaam</t>
-  </si>
-  <si>
     <t>Bericht</t>
   </si>
   <si>
@@ -223,82 +223,13 @@
     <t>Iris</t>
   </si>
   <si>
-    <t>de Jong</t>
-  </si>
-  <si>
-    <t>Jansen</t>
-  </si>
-  <si>
-    <t>de Vries</t>
-  </si>
-  <si>
-    <t>Mulder</t>
-  </si>
-  <si>
-    <t>Bakker</t>
-  </si>
-  <si>
-    <t>Bos</t>
-  </si>
-  <si>
-    <t>Dekker</t>
-  </si>
-  <si>
-    <t>Dijkstra</t>
-  </si>
-  <si>
-    <t>Kok</t>
-  </si>
-  <si>
-    <t>van Vliet</t>
-  </si>
-  <si>
-    <t>van Leeuwen</t>
-  </si>
-  <si>
-    <t>de Groot</t>
-  </si>
-  <si>
-    <t>Veenstra</t>
-  </si>
-  <si>
-    <t>Vink</t>
-  </si>
-  <si>
-    <t>Kuipers</t>
-  </si>
-  <si>
-    <t>Scholten</t>
-  </si>
-  <si>
-    <t>de Lange</t>
-  </si>
-  <si>
-    <t>de Boer</t>
-  </si>
-  <si>
-    <t>Smit</t>
-  </si>
-  <si>
-    <t>Timmerman</t>
-  </si>
-  <si>
-    <t>Hendriks</t>
-  </si>
-  <si>
-    <t>de Graaf</t>
-  </si>
-  <si>
-    <t>van der Linden</t>
-  </si>
-  <si>
-    <t>de Bruijn</t>
-  </si>
-  <si>
-    <t>van den Heuvel</t>
-  </si>
-  <si>
     <t>POI</t>
+  </si>
+  <si>
+    <t>Afbeelding</t>
+  </si>
+  <si>
+    <t>Images/Image.png</t>
   </si>
 </sst>
 </file>
@@ -363,7 +294,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema3">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="data-set">
         <xsd:complexType>
@@ -378,10 +309,10 @@
                           <xsd:complexType>
                             <xsd:sequence minOccurs="0">
                               <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Voornaam" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Achternaam" form="unqualified"/>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Bericht" form="unqualified"/>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="POI" form="unqualified"/>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mediaplatform" form="unqualified"/>
+                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Afbeelding" form="unqualified"/>
                             </xsd:sequence>
                           </xsd:complexType>
                         </xsd:element>
@@ -396,30 +327,30 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="3" Name="data-set_toewijzing" RootElement="data-set" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+  <Map ID="4" Name="data-set_toewijzing" RootElement="data-set" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="4">
   <autoFilter ref="A1:E26" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Voornaam" name="Voornaam">
-      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Voornaam" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{E5E2E653-7318-47D2-9903-41062D660767}" uniqueName="Achternaam" name="Achternaam">
-      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Achternaam" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Voornaam" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Bericht" name="Bericht">
-      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Bericht" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Bericht" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="POI" name="POI" dataDxfId="0">
-      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Mediaplatform" name="Mediaplatform">
-      <xmlColumnPr mapId="3" xpath="/data-set/NotificationCollection/Notifications/Notification/Mediaplatform" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Mediaplatform" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="Afbeelding" name="Afbeelding">
+      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Afbeelding" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -726,15 +657,15 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
-    <col min="5" max="9" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,440 +675,392 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>84</v>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="1">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="1">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
         <v>3</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="1">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Can now load notifications with images
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C72251-A8F3-4390-80CF-C478EF0CD6E8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5606010-AD1D-45B9-A80A-7C7A9F63069D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
@@ -43,18 +43,15 @@
   <connection id="4" xr16:uid="{0ED1EF86-BBAE-4CC0-9C3B-F4D02FDB3F56}" name="Schema3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="5" xr16:uid="{FD7BDC3E-DBB2-49DB-A666-D2FE2F713BB2}" name="Schema4" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
-    <t>Voornaam</t>
-  </si>
-  <si>
-    <t>Bericht</t>
-  </si>
-  <si>
     <t>Is dit al opgelost?</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Nog meer criminaliteit?</t>
   </si>
   <si>
-    <t>Mediaplatform</t>
-  </si>
-  <si>
     <t>SMS</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Twitter</t>
   </si>
   <si>
-    <t>Whattsapp</t>
-  </si>
-  <si>
     <t>Facebook</t>
   </si>
   <si>
@@ -226,10 +217,22 @@
     <t>POI</t>
   </si>
   <si>
-    <t>Afbeelding</t>
-  </si>
-  <si>
-    <t>Images/Image.png</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>PlatformLogoPath</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
   </si>
 </sst>
 </file>
@@ -294,28 +297,22 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema2">
+  <Schema ID="Schema3">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="data-set">
+      <xsd:element nillable="true" name="NotificationCollection">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" name="NotificationCollection" form="unqualified">
+            <xsd:element minOccurs="0" nillable="true" name="Notifications" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" name="Notifications" form="unqualified">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Notification" form="unqualified">
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Notification" form="unqualified">
-                          <xsd:complexType>
-                            <xsd:sequence minOccurs="0">
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Voornaam" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Bericht" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="POI" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mediaplatform" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Afbeelding" form="unqualified"/>
-                            </xsd:sequence>
-                          </xsd:complexType>
-                        </xsd:element>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Message" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="POI" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="PlatformLogoPath" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ImagePath" form="unqualified"/>
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -327,30 +324,30 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="4" Name="data-set_toewijzing" RootElement="data-set" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
+  <Map ID="5" Name="NotificationCollection_toewijzing" RootElement="NotificationCollection" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="5">
   <autoFilter ref="A1:E26" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Voornaam" name="Voornaam">
-      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Voornaam" xmlDataType="string"/>
+    <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Name" name="Name">
+      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Bericht" name="Bericht">
-      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Bericht" xmlDataType="string"/>
+    <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Message" name="Message">
+      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="POI" name="POI" dataDxfId="0">
-      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
+      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Mediaplatform" name="Mediaplatform">
-      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Mediaplatform" xmlDataType="string"/>
+    <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="PlatformLogoPath" name="PlatformLogoPath">
+      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/PlatformLogoPath" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="Afbeelding" name="Afbeelding">
-      <xmlColumnPr mapId="4" xpath="/data-set/NotificationCollection/Notifications/Notification/Afbeelding" xmlDataType="string"/>
+    <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="ImagePath" name="ImagePath">
+      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/ImagePath" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -657,7 +654,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,21 +662,22 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="8" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>59</v>
@@ -687,378 +685,378 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E26" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made XML file names better
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5606010-AD1D-45B9-A80A-7C7A9F63069D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAD092-F527-4D07-BC0E-47D063FAE00A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
@@ -46,11 +46,14 @@
   <connection id="5" xr16:uid="{FD7BDC3E-DBB2-49DB-A666-D2FE2F713BB2}" name="Schema4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="6" xr16:uid="{6F7DD403-1394-4399-9818-E2C388597E37}" name="Schema5" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>Is dit al opgelost?</t>
   </si>
@@ -223,16 +226,13 @@
     <t>Message</t>
   </si>
   <si>
-    <t>PlatformLogoPath</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>ImagePath</t>
-  </si>
-  <si>
     <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>Platform</t>
   </si>
 </sst>
 </file>
@@ -297,7 +297,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema3">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="NotificationCollection">
         <xsd:complexType>
@@ -311,8 +311,8 @@
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Message" form="unqualified"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="POI" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="PlatformLogoPath" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ImagePath" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Platform" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -324,30 +324,30 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="5" Name="NotificationCollection_toewijzing" RootElement="NotificationCollection" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
+  <Map ID="6" Name="NotificationCollection_toewijzing" RootElement="NotificationCollection" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="6">
   <autoFilter ref="A1:E26" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Name" name="Name">
-      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/Name" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/Name" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Message" name="Message">
-      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="POI" name="POI" dataDxfId="0">
-      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
+      <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/POI" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="PlatformLogoPath" name="PlatformLogoPath">
-      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/PlatformLogoPath" xmlDataType="string"/>
+    <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Platform" name="Platform">
+      <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/Platform" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="ImagePath" name="ImagePath">
-      <xmlColumnPr mapId="5" xpath="/NotificationCollection/Notifications/Notification/ImagePath" xmlDataType="string"/>
+    <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="Image" name="Image">
+      <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -654,7 +654,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +677,10 @@
         <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -817,7 +817,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Removed EasyRoads and added extra irrelevant notifications
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\038Games BART VR\BartVR\BartVR\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordyvandenberg/Code/BartVR/Assets/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB32E0D1-B158-48C9-AD72-1ABE8E64C816}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966C6C4A-4818-5E4C-AF59-639685F541DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="28800" windowHeight="12160" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -53,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>Ik zie iemand die zich verdacht gedraagt.</t>
   </si>
@@ -169,24 +164,12 @@
     <t>Ik heb gister een broodje pindakaas gegeten. #peanutbutter4lyfe #lekker</t>
   </si>
   <si>
-    <t>Smash?</t>
-  </si>
-  <si>
-    <t>Fourtnite is leuk #winnerwinnerchickendinner</t>
-  </si>
-  <si>
     <t>#DoeHetVoorGentStudent42.2</t>
   </si>
   <si>
     <t>De bus is weer laat @Synthus #sad #late</t>
   </si>
   <si>
-    <t>Snoepjesgever</t>
-  </si>
-  <si>
-    <t>Iemand een snoepje? #nietXtcHoor</t>
-  </si>
-  <si>
     <t>GentStudent</t>
   </si>
   <si>
@@ -197,6 +180,66 @@
   </si>
   <si>
     <t>VervelendeZeurpiet</t>
+  </si>
+  <si>
+    <t>Waar kan ik de aphotheek vinden?</t>
+  </si>
+  <si>
+    <t>LisaNL12</t>
+  </si>
+  <si>
+    <t>Lekker dagje winkelen met mij vriendinnen!!</t>
+  </si>
+  <si>
+    <t>Wat een mooie dag is het vandaag! Lekker een luchte scheppen :D</t>
+  </si>
+  <si>
+    <t>kopje koffie? Ik krijg er nooit genoeg van!</t>
+  </si>
+  <si>
+    <t>Jordaan038</t>
+  </si>
+  <si>
+    <t>Fluffy06</t>
+  </si>
+  <si>
+    <t>Zag net zo'n schattig knuffeltje. Heb er één gekocht voor mijn broertje maar wil er eigelijk ook zelf één XD</t>
+  </si>
+  <si>
+    <t>Kees1999</t>
+  </si>
+  <si>
+    <t>Dat moment wanneer je niet weet wat je moet tweeten #random</t>
+  </si>
+  <si>
+    <t>Roos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eindelijk klaar met leren! Nu tijd om te relaxen! </t>
+  </si>
+  <si>
+    <t>Ricky4</t>
+  </si>
+  <si>
+    <t>Vandaag ga ik lekker niks doen… behalve dit bericht poste haha</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Whoa kan niet geloven hoe goedkoop die schoenen waren! #lucky #opruiming</t>
+  </si>
+  <si>
+    <t>Sweet Tooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zo hyped!! Buitelands snoep komt morgen binnen!! </t>
+  </si>
+  <si>
+    <t>Marloesje</t>
+  </si>
+  <si>
+    <t>Naar de kapper staat op de planning vandaag! Is ook wel nodig haha</t>
   </si>
 </sst>
 </file>
@@ -295,8 +338,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E18" tableType="xml" totalsRowShown="0" connectionId="6">
-  <autoFilter ref="A1:E18" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:E26" tableType="xml" totalsRowShown="0" connectionId="6">
+  <autoFilter ref="A1:E26" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="6" xpath="/NotificationCollection/Notifications/Notification/Name" xmlDataType="string"/>
@@ -615,22 +658,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35DE26D-FD33-44E6-9F8F-8377B37C5116}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="8" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="8" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -647,7 +690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -664,7 +707,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -679,12 +722,12 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -694,74 +737,72 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -771,57 +812,57 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -831,84 +872,206 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C25" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Able to make list out of base notifications
</commit_message>
<xml_diff>
--- a/Assets/Resources/Berichten.xlsx
+++ b/Assets/Resources/Berichten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\BartVR\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AAE19-0153-4051-8DC0-B0A6178B2766}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CA2A8-0749-4324-91AF-B591CB5F33A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
@@ -32,35 +32,38 @@
   <connection id="2" xr16:uid="{751CB7F7-EAA6-48E0-9A1F-CDEDF00F9B68}" name="Schema1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" xr16:uid="{7C2187DD-9C47-4A30-8977-D2530993B475}" name="Schema2" type="4" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{7B47C04E-4E04-4013-91F0-7272F6608AD6}" name="Schema10" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\Programming\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="4" xr16:uid="{7C2187DD-9C47-4A30-8977-D2530993B475}" name="Schema2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\GitHub\BartVR\Assets\Resources\XML Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" xr16:uid="{0ED1EF86-BBAE-4CC0-9C3B-F4D02FDB3F56}" name="Schema3" type="4" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{0ED1EF86-BBAE-4CC0-9C3B-F4D02FDB3F56}" name="Schema3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" xr16:uid="{FD7BDC3E-DBB2-49DB-A666-D2FE2F713BB2}" name="Schema4" type="4" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{FD7BDC3E-DBB2-49DB-A666-D2FE2F713BB2}" name="Schema4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" xr16:uid="{6F7DD403-1394-4399-9818-E2C388597E37}" name="Schema5" type="4" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{6F7DD403-1394-4399-9818-E2C388597E37}" name="Schema5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\rmast\OneDrive\Documenten\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" xr16:uid="{D1078CE1-0BE8-459D-A8FD-03F5197E67DE}" name="Schema6" type="4" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{D1078CE1-0BE8-459D-A8FD-03F5197E67DE}" name="Schema6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Programming\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" xr16:uid="{CCEFDF45-80C3-4008-94B8-8F6DA38B242C}" name="Schema7" type="4" refreshedVersion="0" background="1">
+  <connection id="9" xr16:uid="{CCEFDF45-80C3-4008-94B8-8F6DA38B242C}" name="Schema7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Programming\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="9" xr16:uid="{445EA795-0822-4028-93A1-88600B7F8C39}" name="Schema8" type="4" refreshedVersion="0" background="1">
+  <connection id="10" xr16:uid="{445EA795-0822-4028-93A1-88600B7F8C39}" name="Schema8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Programming\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="10" xr16:uid="{A0EBD1AB-CCB4-4CAB-8D81-D492E892649B}" name="Schema9" type="4" refreshedVersion="0" background="1">
+  <connection id="11" xr16:uid="{A0EBD1AB-CCB4-4CAB-8D81-D492E892649B}" name="Schema9" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Programming\BartVR\Assets\Resources\XML_Files\Schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>SMS</t>
   </si>
@@ -545,7 +548,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema7">
+  <Schema ID="Schema8">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="NotificationCollection">
         <xsd:complexType>
@@ -553,7 +556,7 @@
             <xsd:element minOccurs="0" nillable="true" name="Notifications" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" name="Notification" form="unqualified">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Notification" form="unqualified">
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
                         <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Id" form="unqualified"/>
@@ -574,36 +577,36 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="11" Name="NotificationCollection_Map" RootElement="NotificationCollection" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="10" DataBindingLoadMode="1"/>
+  <Map ID="12" Name="NotificationCollection_Map" RootElement="NotificationCollection" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:G24" tableType="xml" totalsRowShown="0" connectionId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:G24" tableType="xml" totalsRowShown="0" connectionId="3">
   <autoFilter ref="A1:G24" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="7">
     <tableColumn id="7" xr3:uid="{E954BD75-C2AF-4AB0-A020-84687C11D4B3}" uniqueName="Id" name="Id" dataDxfId="0">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Id" xmlDataType="integer"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Id" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{5566690A-8CE2-4A65-84CB-742B8A242D2A}" uniqueName="ReactionTo" name="ReactionTo" dataDxfId="1">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/ReactionTo" xmlDataType="string"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/ReactionTo" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{53E827BC-24F7-4A2B-A1CA-33B7F4A9621F}" uniqueName="Autor" name="Autor">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Autor" xmlDataType="string"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Autor" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Message" name="Message">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="Image" name="Image" dataDxfId="2">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Image" xmlDataType="string"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Image" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Platform" name="Platform">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Platform" xmlDataType="string"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Platform" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{50E161EE-1C91-4B35-B6A0-9D1FF1983BED}" uniqueName="Postable" name="Postable">
-      <xmlColumnPr mapId="11" xpath="/NotificationCollection/Notifications/Notification/Postable" xmlDataType="boolean"/>
+      <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Postable" xmlDataType="boolean"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -910,7 +913,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1169,9 @@
       <c r="A13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1341,7 +1346,9 @@
       <c r="A22" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>